<commit_message>
remove Hawaii from country list
</commit_message>
<xml_diff>
--- a/AAPI_countries.xlsx
+++ b/AAPI_countries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunnyshao/Documents/immigration_data_clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C7A20A-BCC8-A243-8053-D843750A65DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41054643-0821-B347-9392-889A86725244}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7260" yWindow="3580" windowWidth="27240" windowHeight="16440" xr2:uid="{90067342-255C-BB47-BAE9-3E7AD111EFF9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>asian_country</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>India</t>
-  </si>
-  <si>
-    <t>Hawaii</t>
   </si>
   <si>
     <t>Indonesia</t>
@@ -493,7 +490,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -566,93 +563,90 @@
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>